<commit_message>
Added FollowUp ECAS columns to Progeny query (found in Netherlands/Harold/20180214_MRI Also used 'ALS number' instead of 'ALSnummer #'
Increased value of read_excel(guess_max) to an arbitrary large number (default of 1000 is not enough)
</commit_message>
<xml_diff>
--- a/Data/Format_v1.xlsx
+++ b/Data/Format_v1.xlsx
@@ -1,19 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Promise_Pegasus/Harold/Rprojects/MRI/Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="400" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21940" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$57</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +33,7 @@
     <author>Henk-Jan Westeneng</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B2" authorId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -76,7 +81,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0">
+    <comment ref="H2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -110,7 +115,7 @@
     <author>Henk-Jan Westeneng</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -135,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0">
+    <comment ref="C6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -159,7 +164,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D6" authorId="0">
+    <comment ref="D6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -188,7 +193,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="142">
   <si>
     <t>Original</t>
   </si>
@@ -208,9 +213,6 @@
     <t>Possible_values</t>
   </si>
   <si>
-    <t>ALSnummer #</t>
-  </si>
-  <si>
     <t>ALSnr</t>
   </si>
   <si>
@@ -274,24 +276,15 @@
     <t>ECAS_Total_Score</t>
   </si>
   <si>
-    <t>ECAS_total</t>
-  </si>
-  <si>
     <t>numeric</t>
   </si>
   <si>
     <t>ECAS ALS_SPECIFIC</t>
   </si>
   <si>
-    <t>ECAS_spec</t>
-  </si>
-  <si>
     <t>ECAS ALS_NONSPECIFIC</t>
   </si>
   <si>
-    <t>ECAS_nonspec</t>
-  </si>
-  <si>
     <t>ECAS: Date of testing</t>
   </si>
   <si>
@@ -394,9 +387,6 @@
     <t>ECAS: Version A or B</t>
   </si>
   <si>
-    <t>ECAS_version</t>
-  </si>
-  <si>
     <t>Bulbar|Spinal|Thoracic/respiratory|Generalized</t>
   </si>
   <si>
@@ -461,12 +451,180 @@
   </si>
   <si>
     <t>Dit is de identifier (altijd Group==ID geven). Voor ID ip altijd Regex gebruiken (nooit min, max of possible values).</t>
+  </si>
+  <si>
+    <t>FU2: ECAS: Date of testing</t>
+  </si>
+  <si>
+    <t>FU3: ECAS: Date of testing</t>
+  </si>
+  <si>
+    <t>FU4: ECAS: Date of testing</t>
+  </si>
+  <si>
+    <t>FU5: ECAS: Date of testing</t>
+  </si>
+  <si>
+    <t>FU2 ECAS: Version A or B</t>
+  </si>
+  <si>
+    <t>FU3 ECAS: Version A or B</t>
+  </si>
+  <si>
+    <t>FU4 ECAS: Version A or B</t>
+  </si>
+  <si>
+    <t>FU5 ECAS: Version A or B</t>
+  </si>
+  <si>
+    <t>Reat or write problems</t>
+  </si>
+  <si>
+    <t>FU2: Read or write problems</t>
+  </si>
+  <si>
+    <t>FU3: Read or write problems</t>
+  </si>
+  <si>
+    <t>FU4: Read or write problems</t>
+  </si>
+  <si>
+    <t>FU5: Read or write problems</t>
+  </si>
+  <si>
+    <t>FU2: ECAS ALS_SPECIFIC</t>
+  </si>
+  <si>
+    <t>FU3: ECAS ALS_SPECIFIC</t>
+  </si>
+  <si>
+    <t>FU4: ECAS ALS_SPECIFIC</t>
+  </si>
+  <si>
+    <t>FU5: ECAS ALS_SPECIFIC</t>
+  </si>
+  <si>
+    <t>FU2: ECAS ALS_NONSPECIFIC</t>
+  </si>
+  <si>
+    <t>FU3: ECAS ALS_NONSPECIFIC</t>
+  </si>
+  <si>
+    <t>FU4: ECAS ALS-NONSPECIFIC</t>
+  </si>
+  <si>
+    <t>FU5: ECAS ALS_NONSPECIFIC</t>
+  </si>
+  <si>
+    <t>FU2: ECAS Total score</t>
+  </si>
+  <si>
+    <t>FU3: ECAS Total score</t>
+  </si>
+  <si>
+    <t>FU4: ECAS Total score</t>
+  </si>
+  <si>
+    <t>FU5: ECAS Total score</t>
+  </si>
+  <si>
+    <t>DoECAS1</t>
+  </si>
+  <si>
+    <t>DoECAS2</t>
+  </si>
+  <si>
+    <t>DoECAS3</t>
+  </si>
+  <si>
+    <t>DoECAS4</t>
+  </si>
+  <si>
+    <t>DoECAS5</t>
+  </si>
+  <si>
+    <t>ECAS_version1</t>
+  </si>
+  <si>
+    <t>ECAS_version2</t>
+  </si>
+  <si>
+    <t>ECAS_version3</t>
+  </si>
+  <si>
+    <t>ECAS_version4</t>
+  </si>
+  <si>
+    <t>ECAS_version5</t>
+  </si>
+  <si>
+    <t>ECAS_problemrw1</t>
+  </si>
+  <si>
+    <t>ECAS_problemrw2</t>
+  </si>
+  <si>
+    <t>ECAS_problemrw3</t>
+  </si>
+  <si>
+    <t>ECAS_problemrw4</t>
+  </si>
+  <si>
+    <t>ECAS_problemrw5</t>
+  </si>
+  <si>
+    <t>ECAS_spec1</t>
+  </si>
+  <si>
+    <t>ECAS_spec2</t>
+  </si>
+  <si>
+    <t>ECAS_spec3</t>
+  </si>
+  <si>
+    <t>ECAS_spec4</t>
+  </si>
+  <si>
+    <t>ECAS_spec5</t>
+  </si>
+  <si>
+    <t>ECAS_nonspec1</t>
+  </si>
+  <si>
+    <t>ECAS_nonspec2</t>
+  </si>
+  <si>
+    <t>ECAS_nonspec3</t>
+  </si>
+  <si>
+    <t>ECAS_nonspec4</t>
+  </si>
+  <si>
+    <t>ECAS_nonspec5</t>
+  </si>
+  <si>
+    <t>ECAS_total1</t>
+  </si>
+  <si>
+    <t>ECAS_total2</t>
+  </si>
+  <si>
+    <t>ECAS_total3</t>
+  </si>
+  <si>
+    <t>ECAS_total4</t>
+  </si>
+  <si>
+    <t>ECAS_total5</t>
+  </si>
+  <si>
+    <t>ALS number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -679,6 +837,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1004,16 +1170,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
@@ -1022,7 +1188,7 @@
     <col min="8" max="9" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1042,635 +1208,1131 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
       <c r="G2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
       </c>
       <c r="D4" s="2">
         <v>367</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2">
         <v>18264</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="2">
         <v>18264</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="2">
         <v>29221</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="2">
         <v>29221</v>
       </c>
       <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="2">
+        <v>40179</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="2">
+        <v>40180</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="2">
+        <v>40181</v>
+      </c>
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="2">
+        <v>40182</v>
+      </c>
+      <c r="E14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="2">
+        <v>40183</v>
+      </c>
+      <c r="E15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="F16" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17" t="s">
+        <v>80</v>
+      </c>
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18" t="s">
+        <v>80</v>
+      </c>
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" t="s">
+        <v>80</v>
+      </c>
+      <c r="I19" s="7"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" t="s">
+        <v>67</v>
+      </c>
+      <c r="H20" t="s">
+        <v>80</v>
+      </c>
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="5"/>
+      <c r="H21" t="s">
+        <v>80</v>
+      </c>
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" t="s">
+        <v>122</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="5"/>
+      <c r="H22" t="s">
+        <v>80</v>
+      </c>
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" t="s">
+        <v>123</v>
+      </c>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="5"/>
+      <c r="H23" t="s">
+        <v>80</v>
+      </c>
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" t="s">
+        <v>124</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="5"/>
+      <c r="H24" t="s">
+        <v>80</v>
+      </c>
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="5"/>
+      <c r="H25" t="s">
+        <v>80</v>
+      </c>
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
+        <v>126</v>
+      </c>
+      <c r="C26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="5">
+        <v>0</v>
+      </c>
+      <c r="E26" s="5">
+        <v>100</v>
+      </c>
+      <c r="H26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" t="s">
+        <v>127</v>
+      </c>
+      <c r="C27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="5">
+        <v>0</v>
+      </c>
+      <c r="E27" s="5">
+        <v>100</v>
+      </c>
+      <c r="F27" s="5"/>
+      <c r="H27" t="s">
+        <v>80</v>
+      </c>
+      <c r="I27" s="7"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" t="s">
+        <v>128</v>
+      </c>
+      <c r="C28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="5">
+        <v>0</v>
+      </c>
+      <c r="E28" s="5">
+        <v>100</v>
+      </c>
+      <c r="F28" s="5"/>
+      <c r="H28" t="s">
+        <v>80</v>
+      </c>
+      <c r="I28" s="7"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" t="s">
+        <v>129</v>
+      </c>
+      <c r="C29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="5">
+        <v>0</v>
+      </c>
+      <c r="E29" s="5">
+        <v>100</v>
+      </c>
+      <c r="F29" s="5"/>
+      <c r="H29" t="s">
+        <v>80</v>
+      </c>
+      <c r="I29" s="7"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>102</v>
+      </c>
+      <c r="B30" t="s">
+        <v>130</v>
+      </c>
+      <c r="C30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="5">
+        <v>0</v>
+      </c>
+      <c r="E30" s="5">
+        <v>100</v>
+      </c>
+      <c r="F30" s="5"/>
+      <c r="H30" t="s">
+        <v>80</v>
+      </c>
+      <c r="I30" s="7"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>131</v>
+      </c>
+      <c r="C31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="5">
+        <v>0</v>
+      </c>
+      <c r="E31" s="5">
+        <v>36</v>
+      </c>
+      <c r="H31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>103</v>
+      </c>
+      <c r="B32" t="s">
+        <v>132</v>
+      </c>
+      <c r="C32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="5">
+        <v>0</v>
+      </c>
+      <c r="E32" s="5">
+        <v>36</v>
+      </c>
+      <c r="F32" s="5"/>
+      <c r="H32" t="s">
+        <v>80</v>
+      </c>
+      <c r="I32" s="7"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" t="s">
+        <v>133</v>
+      </c>
+      <c r="C33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="5">
+        <v>0</v>
+      </c>
+      <c r="E33" s="5">
+        <v>36</v>
+      </c>
+      <c r="F33" s="5"/>
+      <c r="H33" t="s">
+        <v>80</v>
+      </c>
+      <c r="I33" s="7"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" t="s">
+        <v>134</v>
+      </c>
+      <c r="C34" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="5">
+        <v>0</v>
+      </c>
+      <c r="E34" s="5">
+        <v>36</v>
+      </c>
+      <c r="F34" s="5"/>
+      <c r="H34" t="s">
+        <v>80</v>
+      </c>
+      <c r="I34" s="7"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35" t="s">
+        <v>135</v>
+      </c>
+      <c r="C35" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="5">
+        <v>0</v>
+      </c>
+      <c r="E35" s="5">
+        <v>36</v>
+      </c>
+      <c r="F35" s="5"/>
+      <c r="H35" t="s">
+        <v>80</v>
+      </c>
+      <c r="I35" s="7"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>26</v>
       </c>
-      <c r="H8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" t="s">
+      <c r="B36" t="s">
+        <v>136</v>
+      </c>
+      <c r="C36" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="5">
+        <v>0</v>
+      </c>
+      <c r="E36" s="5">
+        <v>136</v>
+      </c>
+      <c r="H36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>107</v>
+      </c>
+      <c r="B37" t="s">
+        <v>137</v>
+      </c>
+      <c r="C37" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" s="5">
+        <v>0</v>
+      </c>
+      <c r="E37" s="5">
+        <v>136</v>
+      </c>
+      <c r="F37" s="5"/>
+      <c r="H37" t="s">
+        <v>80</v>
+      </c>
+      <c r="I37" s="7"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" t="s">
+        <v>138</v>
+      </c>
+      <c r="C38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D38" s="5">
+        <v>0</v>
+      </c>
+      <c r="E38" s="5">
+        <v>136</v>
+      </c>
+      <c r="F38" s="5"/>
+      <c r="H38" t="s">
+        <v>80</v>
+      </c>
+      <c r="I38" s="7"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" t="s">
+        <v>139</v>
+      </c>
+      <c r="C39" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="5">
+        <v>0</v>
+      </c>
+      <c r="E39" s="5">
+        <v>136</v>
+      </c>
+      <c r="F39" s="5"/>
+      <c r="H39" t="s">
+        <v>80</v>
+      </c>
+      <c r="I39" s="7"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40" t="s">
+        <v>140</v>
+      </c>
+      <c r="C40" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" s="5">
+        <v>0</v>
+      </c>
+      <c r="E40" s="5">
+        <v>136</v>
+      </c>
+      <c r="F40" s="5"/>
+      <c r="H40" t="s">
+        <v>80</v>
+      </c>
+      <c r="I40" s="7"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="2">
+        <v>32874</v>
+      </c>
+      <c r="E41" t="s">
+        <v>25</v>
+      </c>
+      <c r="H41" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>4</v>
+      </c>
+      <c r="H42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" t="s">
+        <v>27</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>4</v>
+      </c>
+      <c r="H43" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" t="s">
+        <v>39</v>
+      </c>
+      <c r="C44" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>4</v>
+      </c>
+      <c r="H44" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>40</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45" t="s">
+        <v>27</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>4</v>
+      </c>
+      <c r="H45" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C46" t="s">
+        <v>27</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>4</v>
+      </c>
+      <c r="H46" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" t="s">
+        <v>27</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>4</v>
+      </c>
+      <c r="H47" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>47</v>
+      </c>
+      <c r="C48" t="s">
+        <v>27</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>4</v>
+      </c>
+      <c r="H48" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49" t="s">
+        <v>27</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>4</v>
+      </c>
+      <c r="H49" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50" t="s">
+        <v>27</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>4</v>
+      </c>
+      <c r="H50" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51" t="s">
+        <v>27</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>4</v>
+      </c>
+      <c r="H51" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52" t="s">
+        <v>27</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>4</v>
+      </c>
+      <c r="H52" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C53" t="s">
+        <v>27</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>4</v>
+      </c>
+      <c r="H53" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>58</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C54" t="s">
+        <v>27</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>4</v>
+      </c>
+      <c r="H54" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C55" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" s="2">
+        <v>29221</v>
+      </c>
+      <c r="E55" t="s">
+        <v>25</v>
+      </c>
+      <c r="H55" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>72</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C56" t="s">
+        <v>27</v>
+      </c>
+      <c r="D56">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="E56">
+        <v>200</v>
+      </c>
+      <c r="H56" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C57" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="H9" s="7" t="s">
+      <c r="D57" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H57" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="5">
-        <v>0</v>
-      </c>
-      <c r="E11" s="5">
-        <v>136</v>
-      </c>
-      <c r="H11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="5">
-        <v>0</v>
-      </c>
-      <c r="E12" s="5">
-        <v>100</v>
-      </c>
-      <c r="H12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="5">
-        <v>0</v>
-      </c>
-      <c r="E13" s="5">
-        <v>36</v>
-      </c>
-      <c r="H13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="2">
-        <v>40179</v>
-      </c>
-      <c r="E14" t="s">
-        <v>26</v>
-      </c>
-      <c r="H14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="F15" t="s">
-        <v>72</v>
-      </c>
-      <c r="H15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="2">
-        <v>32874</v>
-      </c>
-      <c r="E16" t="s">
-        <v>26</v>
-      </c>
-      <c r="H16" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>4</v>
-      </c>
-      <c r="H17" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>4</v>
-      </c>
-      <c r="H18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>4</v>
-      </c>
-      <c r="H19" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>4</v>
-      </c>
-      <c r="H20" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>4</v>
-      </c>
-      <c r="H21" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>4</v>
-      </c>
-      <c r="H22" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>4</v>
-      </c>
-      <c r="H23" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>4</v>
-      </c>
-      <c r="H24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>4</v>
-      </c>
-      <c r="H25" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>4</v>
-      </c>
-      <c r="H26" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>4</v>
-      </c>
-      <c r="H27" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" t="s">
-        <v>60</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>4</v>
-      </c>
-      <c r="H28" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" t="s">
-        <v>62</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>4</v>
-      </c>
-      <c r="H29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C30" t="s">
-        <v>14</v>
-      </c>
-      <c r="D30" s="2">
-        <v>29221</v>
-      </c>
-      <c r="E30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H30" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" t="s">
-        <v>77</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C31" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31">
-        <v>20</v>
-      </c>
-      <c r="E31">
-        <v>200</v>
-      </c>
-      <c r="H31" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" t="s">
-        <v>73</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C32" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="I32" s="4"/>
+      <c r="I57" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1688,13 +2350,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
       <c r="B1" s="1" t="str">
         <f>A2</f>
@@ -1729,24 +2391,24 @@
         <v>DoFVC</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="8"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>-1</v>
       </c>
       <c r="C3" s="8"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>-1</v>
@@ -1756,9 +2418,9 @@
       </c>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B5">
         <v>-1</v>
@@ -1771,9 +2433,9 @@
       </c>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B6">
         <v>-1</v>
@@ -1782,9 +2444,9 @@
       <c r="D6" s="4"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B7">
         <v>-1</v>
@@ -1794,9 +2456,9 @@
       </c>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>-1</v>
@@ -1809,9 +2471,9 @@
       </c>
       <c r="H8" s="8"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B9">
         <v>-1</v>

</xml_diff>

<commit_message>
Wide2Long opgelost en geimplementeerd
To do:
formatting
extra check inbouwen
</commit_message>
<xml_diff>
--- a/Data/Format_v1.xlsx
+++ b/Data/Format_v1.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10116"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Promise_Pegasus/Harold/Rprojects/MRI/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/htan4/Documents/Rprojects/MRI/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21940" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21940" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$57</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -193,7 +193,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="142">
   <si>
     <t>Original</t>
   </si>
@@ -1172,8 +1172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1430,7 +1430,9 @@
         <v>25</v>
       </c>
       <c r="F12" s="5"/>
-      <c r="H12" s="7"/>
+      <c r="H12" t="s">
+        <v>80</v>
+      </c>
       <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -1450,7 +1452,9 @@
         <v>25</v>
       </c>
       <c r="F13" s="5"/>
-      <c r="H13" s="7"/>
+      <c r="H13" t="s">
+        <v>80</v>
+      </c>
       <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -1470,7 +1474,9 @@
         <v>25</v>
       </c>
       <c r="F14" s="5"/>
-      <c r="H14" s="7"/>
+      <c r="H14" t="s">
+        <v>80</v>
+      </c>
       <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -1490,7 +1496,9 @@
         <v>25</v>
       </c>
       <c r="F15" s="5"/>
-      <c r="H15" s="7"/>
+      <c r="H15" t="s">
+        <v>80</v>
+      </c>
       <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Voeg uitleg toe nav #3 en #8
</commit_message>
<xml_diff>
--- a/Data/Format_v1.xlsx
+++ b/Data/Format_v1.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/htan4/Documents/Rprojects/MRI/Data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="21940" windowHeight="16000" tabRatio="500"/>
   </bookViews>
@@ -33,7 +28,7 @@
     <author>Henk-Jan Westeneng</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -53,11 +48,36 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Is van belang om juiste naam een longitudinale data te geven.</t>
+Voor variabelen die in wide format staan, terwijl het eigenlijk om long data gaat, is het uitermate belangrijk om de "Rename" zo te kiezen dat er slechts 1 letter/1 cijfer verschil is tussen de verschillende renames.
+@Harold: schrijf jij nog iets in deze comment over supergroepen? Daar moet denk ik ook rekening mee gehouden worden in de rename toch?</t>
         </r>
       </text>
     </comment>
-    <comment ref="B2" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Henk-Jan Westeneng:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Is van belang om juiste naam aan longitudinale data te geven.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -81,7 +101,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0" shapeId="0">
+    <comment ref="H2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -115,7 +135,7 @@
     <author>Henk-Jan Westeneng</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -140,7 +160,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0" shapeId="0">
+    <comment ref="C6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -164,7 +184,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D6" authorId="0" shapeId="0">
+    <comment ref="D6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -624,7 +644,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1172,11 +1192,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11:H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="50.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
@@ -1188,7 +1208,7 @@
     <col min="8" max="9" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1220,7 +1240,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>141</v>
       </c>
@@ -1240,7 +1260,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1257,7 +1277,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1277,7 +1297,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1297,7 +1317,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1317,7 +1337,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1337,7 +1357,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -1357,7 +1377,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1375,7 +1395,7 @@
       </c>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1393,7 +1413,7 @@
       </c>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1413,7 +1433,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>86</v>
       </c>
@@ -1435,7 +1455,7 @@
       </c>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>87</v>
       </c>
@@ -1457,7 +1477,7 @@
       </c>
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>88</v>
       </c>
@@ -1479,7 +1499,7 @@
       </c>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>89</v>
       </c>
@@ -1501,7 +1521,7 @@
       </c>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -1519,7 +1539,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>90</v>
       </c>
@@ -1537,7 +1557,7 @@
       </c>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>91</v>
       </c>
@@ -1555,7 +1575,7 @@
       </c>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>92</v>
       </c>
@@ -1573,7 +1593,7 @@
       </c>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>93</v>
       </c>
@@ -1591,7 +1611,7 @@
       </c>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>94</v>
       </c>
@@ -1607,7 +1627,7 @@
       </c>
       <c r="I21" s="7"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>95</v>
       </c>
@@ -1623,7 +1643,7 @@
       </c>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>96</v>
       </c>
@@ -1639,7 +1659,7 @@
       </c>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>97</v>
       </c>
@@ -1655,7 +1675,7 @@
       </c>
       <c r="I24" s="7"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>98</v>
       </c>
@@ -1671,7 +1691,7 @@
       </c>
       <c r="I25" s="7"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1691,7 +1711,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>99</v>
       </c>
@@ -1713,7 +1733,7 @@
       </c>
       <c r="I27" s="7"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>100</v>
       </c>
@@ -1735,7 +1755,7 @@
       </c>
       <c r="I28" s="7"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>101</v>
       </c>
@@ -1757,7 +1777,7 @@
       </c>
       <c r="I29" s="7"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>102</v>
       </c>
@@ -1779,7 +1799,7 @@
       </c>
       <c r="I30" s="7"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1799,7 +1819,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>103</v>
       </c>
@@ -1821,7 +1841,7 @@
       </c>
       <c r="I32" s="7"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
         <v>104</v>
       </c>
@@ -1843,7 +1863,7 @@
       </c>
       <c r="I33" s="7"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>105</v>
       </c>
@@ -1865,7 +1885,7 @@
       </c>
       <c r="I34" s="7"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>106</v>
       </c>
@@ -1887,7 +1907,7 @@
       </c>
       <c r="I35" s="7"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
         <v>26</v>
       </c>
@@ -1907,7 +1927,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
         <v>107</v>
       </c>
@@ -1929,7 +1949,7 @@
       </c>
       <c r="I37" s="7"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
         <v>108</v>
       </c>
@@ -1951,7 +1971,7 @@
       </c>
       <c r="I38" s="7"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
         <v>109</v>
       </c>
@@ -1973,7 +1993,7 @@
       </c>
       <c r="I39" s="7"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
         <v>110</v>
       </c>
@@ -1995,7 +2015,7 @@
       </c>
       <c r="I40" s="7"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
         <v>32</v>
       </c>
@@ -2015,7 +2035,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
         <v>34</v>
       </c>
@@ -2035,7 +2055,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
         <v>36</v>
       </c>
@@ -2055,7 +2075,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
         <v>38</v>
       </c>
@@ -2075,7 +2095,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
         <v>40</v>
       </c>
@@ -2095,7 +2115,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9">
       <c r="A46" t="s">
         <v>42</v>
       </c>
@@ -2115,7 +2135,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9">
       <c r="A47" t="s">
         <v>44</v>
       </c>
@@ -2135,7 +2155,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -2155,7 +2175,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -2175,7 +2195,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -2195,7 +2215,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -2215,7 +2235,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9">
       <c r="A52" t="s">
         <v>54</v>
       </c>
@@ -2235,7 +2255,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -2255,7 +2275,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9">
       <c r="A54" t="s">
         <v>58</v>
       </c>
@@ -2275,7 +2295,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9">
       <c r="A55" s="6" t="s">
         <v>71</v>
       </c>
@@ -2295,7 +2315,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9">
       <c r="A56" t="s">
         <v>72</v>
       </c>
@@ -2315,7 +2335,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9">
       <c r="A57" t="s">
         <v>68</v>
       </c>
@@ -2362,9 +2382,9 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="4"/>
       <c r="B1" s="1" t="str">
         <f>A2</f>
@@ -2399,13 +2419,13 @@
         <v>DoFVC</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="8"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="9" t="s">
         <v>15</v>
       </c>
@@ -2414,7 +2434,7 @@
       </c>
       <c r="C3" s="8"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="9" t="s">
         <v>17</v>
       </c>
@@ -2426,7 +2446,7 @@
       </c>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="9" t="s">
         <v>70</v>
       </c>
@@ -2441,7 +2461,7 @@
       </c>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="9" t="s">
         <v>62</v>
       </c>
@@ -2452,7 +2472,7 @@
       <c r="D6" s="4"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="9" t="s">
         <v>31</v>
       </c>
@@ -2464,7 +2484,7 @@
       </c>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" s="9" t="s">
         <v>33</v>
       </c>
@@ -2479,7 +2499,7 @@
       </c>
       <c r="H8" s="8"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" s="10" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
Review van code, onnodige unlist() weggehaald (niet meer nodig na nieuwe manier van mergen hier3) Ziet er goed uit HJ!
</commit_message>
<xml_diff>
--- a/Data/Format_v1.xlsx
+++ b/Data/Format_v1.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10116"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/htan4/Documents/Rprojects/MRI/Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21940" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$57</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,13 +33,13 @@
     <author>Henk-Jan Westeneng</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
@@ -43,23 +48,71 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Voor variabelen die in wide format staan, terwijl het eigenlijk om long data gaat, is het uitermate belangrijk om de "Rename" zo te kiezen dat er slechts 1 cijfer verschil is tussen de verschillende renames.
-@Harold: schrijf jij nog iets in deze comment over supergroepen? Daar moet denk ik ook rekening mee gehouden worden in de rename toch?</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Voor variabelen die in wide format staan, terwijl het eigenlijk om long data gaat, is het uitermate belangrijk om de "Rename" zo te kiezen dat er slechts 1 letter/1 cijfer verschil is tussen de verschillende renames.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Voor wide2long variabelen gelden 2 regels:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">1. Binnen elke subgroep mag de "Rename" slechts met 1 cijfer verschillen.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>2. De tags voor de supergroep binnen "Rename" mag nooit korter zijn dan de bijbehorende aanduiding onder kolom "Group"</t>
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
@@ -68,22 +121,51 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Is van belang om juiste naam aan longitudinale data te geven.</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Is van belang om juiste naam aan longitudinale data te geven.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Voor wide 2 long variabelen geldt dat "Group" nooit langer mag zijn dan de bijbehorende tags in de "Rename"  kolom.</t>
         </r>
       </text>
     </comment>
-    <comment ref="B2" authorId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
@@ -92,22 +174,31 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Rename van identifier moet altijd ALSnr zijn.</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rename van identifier moet altijd ALSnr zijn.</t>
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0">
+    <comment ref="H2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
@@ -116,12 +207,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Script is niet getest voor &gt;1 identifier! Dus ip "ID" maar bij 1 cel invullen.</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Script is niet getest voor &gt;1 identifier! Dus ip "ID" maar bij 1 cel invullen.</t>
         </r>
       </text>
     </comment>
@@ -135,7 +235,7 @@
     <author>Henk-Jan Westeneng</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -160,7 +260,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0">
+    <comment ref="C6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -184,7 +284,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D6" authorId="0">
+    <comment ref="D6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -644,8 +744,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -721,6 +821,19 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1193,22 +1306,22 @@
   <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="40.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1240,7 +1353,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>141</v>
       </c>
@@ -1260,7 +1373,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1277,7 +1390,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1297,7 +1410,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1317,7 +1430,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1337,7 +1450,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1357,7 +1470,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -1377,7 +1490,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1395,7 +1508,7 @@
       </c>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1413,7 +1526,7 @@
       </c>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1433,7 +1546,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>86</v>
       </c>
@@ -1444,7 +1557,7 @@
         <v>13</v>
       </c>
       <c r="D12" s="2">
-        <v>40180</v>
+        <v>40179</v>
       </c>
       <c r="E12" t="s">
         <v>25</v>
@@ -1455,7 +1568,7 @@
       </c>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>87</v>
       </c>
@@ -1466,7 +1579,7 @@
         <v>13</v>
       </c>
       <c r="D13" s="2">
-        <v>40181</v>
+        <v>40179</v>
       </c>
       <c r="E13" t="s">
         <v>25</v>
@@ -1477,7 +1590,7 @@
       </c>
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>88</v>
       </c>
@@ -1488,7 +1601,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="2">
-        <v>40182</v>
+        <v>40179</v>
       </c>
       <c r="E14" t="s">
         <v>25</v>
@@ -1499,7 +1612,7 @@
       </c>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>89</v>
       </c>
@@ -1510,7 +1623,7 @@
         <v>13</v>
       </c>
       <c r="D15" s="2">
-        <v>40183</v>
+        <v>40179</v>
       </c>
       <c r="E15" t="s">
         <v>25</v>
@@ -1521,7 +1634,7 @@
       </c>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -1539,7 +1652,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>90</v>
       </c>
@@ -1557,7 +1670,7 @@
       </c>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>91</v>
       </c>
@@ -1575,7 +1688,7 @@
       </c>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>92</v>
       </c>
@@ -1593,7 +1706,7 @@
       </c>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>93</v>
       </c>
@@ -1611,7 +1724,7 @@
       </c>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>94</v>
       </c>
@@ -1627,7 +1740,7 @@
       </c>
       <c r="I21" s="7"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>95</v>
       </c>
@@ -1643,7 +1756,7 @@
       </c>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>96</v>
       </c>
@@ -1659,7 +1772,7 @@
       </c>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>97</v>
       </c>
@@ -1675,7 +1788,7 @@
       </c>
       <c r="I24" s="7"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>98</v>
       </c>
@@ -1691,7 +1804,7 @@
       </c>
       <c r="I25" s="7"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1711,7 +1824,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>99</v>
       </c>
@@ -1733,7 +1846,7 @@
       </c>
       <c r="I27" s="7"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>100</v>
       </c>
@@ -1755,7 +1868,7 @@
       </c>
       <c r="I28" s="7"/>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>101</v>
       </c>
@@ -1777,7 +1890,7 @@
       </c>
       <c r="I29" s="7"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>102</v>
       </c>
@@ -1799,7 +1912,7 @@
       </c>
       <c r="I30" s="7"/>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1819,7 +1932,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>103</v>
       </c>
@@ -1841,7 +1954,7 @@
       </c>
       <c r="I32" s="7"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>104</v>
       </c>
@@ -1863,7 +1976,7 @@
       </c>
       <c r="I33" s="7"/>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>105</v>
       </c>
@@ -1885,7 +1998,7 @@
       </c>
       <c r="I34" s="7"/>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>106</v>
       </c>
@@ -1907,7 +2020,7 @@
       </c>
       <c r="I35" s="7"/>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>26</v>
       </c>
@@ -1927,7 +2040,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>107</v>
       </c>
@@ -1949,7 +2062,7 @@
       </c>
       <c r="I37" s="7"/>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>108</v>
       </c>
@@ -1971,7 +2084,7 @@
       </c>
       <c r="I38" s="7"/>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>109</v>
       </c>
@@ -1993,7 +2106,7 @@
       </c>
       <c r="I39" s="7"/>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>110</v>
       </c>
@@ -2015,7 +2128,7 @@
       </c>
       <c r="I40" s="7"/>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>32</v>
       </c>
@@ -2035,7 +2148,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>34</v>
       </c>
@@ -2055,7 +2168,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>36</v>
       </c>
@@ -2075,7 +2188,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>38</v>
       </c>
@@ -2095,7 +2208,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>40</v>
       </c>
@@ -2115,7 +2228,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>42</v>
       </c>
@@ -2135,7 +2248,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>44</v>
       </c>
@@ -2155,7 +2268,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -2175,7 +2288,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -2195,7 +2308,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -2215,7 +2328,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -2235,7 +2348,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>54</v>
       </c>
@@ -2255,7 +2368,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -2275,7 +2388,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>58</v>
       </c>
@@ -2295,7 +2408,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>71</v>
       </c>
@@ -2315,7 +2428,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>72</v>
       </c>
@@ -2335,7 +2448,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>68</v>
       </c>
@@ -2382,9 +2495,9 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
       <c r="B1" s="1" t="str">
         <f>A2</f>
@@ -2419,13 +2532,13 @@
         <v>DoFVC</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="8"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>15</v>
       </c>
@@ -2434,7 +2547,7 @@
       </c>
       <c r="C3" s="8"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>17</v>
       </c>
@@ -2446,7 +2559,7 @@
       </c>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>70</v>
       </c>
@@ -2461,7 +2574,7 @@
       </c>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>62</v>
       </c>
@@ -2472,7 +2585,7 @@
       <c r="D6" s="4"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>31</v>
       </c>
@@ -2484,7 +2597,7 @@
       </c>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>33</v>
       </c>
@@ -2499,7 +2612,7 @@
       </c>
       <c r="H8" s="8"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
Comments aangepast zoals in #9. Tevens minimum waardes voor DoECAS aangepast.
</commit_message>
<xml_diff>
--- a/Data/Format_v1.xlsx
+++ b/Data/Format_v1.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10116"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/htan4/Documents/Rprojects/MRI/Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21940" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$57</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,13 +33,13 @@
     <author>Henk-Jan Westeneng</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
@@ -43,23 +48,71 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Voor variabelen die in wide format staan, terwijl het eigenlijk om long data gaat, is het uitermate belangrijk om de "Rename" zo te kiezen dat er slechts 1 cijfer verschil is tussen de verschillende renames.
-@Harold: schrijf jij nog iets in deze comment over supergroepen? Daar moet denk ik ook rekening mee gehouden worden in de rename toch?</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Voor variabelen die in wide format staan, terwijl het eigenlijk om long data gaat, is het uitermate belangrijk om de "Rename" zo te kiezen dat er slechts 1 letter/1 cijfer verschil is tussen de verschillende renames.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Voor wide2long variabelen gelden 2 regels:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">1. Binnen elke subgroep mag de "Rename" slechts met 1 cijfer verschillen.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>2. De tags voor de supergroep binnen "Rename" mag nooit korter zijn dan de bijbehorende aanduiding onder kolom "Group"</t>
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
@@ -68,22 +121,51 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Is van belang om juiste naam aan longitudinale data te geven.</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Is van belang om juiste naam aan longitudinale data te geven.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Voor wide 2 long variabelen geldt dat "Group" nooit langer mag zijn dan de bijbehorende tags in de "Rename"  kolom.</t>
         </r>
       </text>
     </comment>
-    <comment ref="B2" authorId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
@@ -92,22 +174,31 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Rename van identifier moet altijd ALSnr zijn.</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rename van identifier moet altijd ALSnr zijn.</t>
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0">
+    <comment ref="H2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
@@ -116,12 +207,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Script is niet getest voor &gt;1 identifier! Dus ip "ID" maar bij 1 cel invullen.</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Script is niet getest voor &gt;1 identifier! Dus ip "ID" maar bij 1 cel invullen.</t>
         </r>
       </text>
     </comment>
@@ -135,7 +235,7 @@
     <author>Henk-Jan Westeneng</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -160,7 +260,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0">
+    <comment ref="C6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -184,7 +284,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D6" authorId="0">
+    <comment ref="D6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -644,8 +744,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -721,6 +821,19 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1193,22 +1306,22 @@
   <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="40.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1240,7 +1353,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>141</v>
       </c>
@@ -1260,7 +1373,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1277,7 +1390,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1297,7 +1410,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1317,7 +1430,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1337,7 +1450,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1357,7 +1470,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -1377,7 +1490,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1395,7 +1508,7 @@
       </c>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1413,7 +1526,7 @@
       </c>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1433,7 +1546,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>86</v>
       </c>
@@ -1444,7 +1557,7 @@
         <v>13</v>
       </c>
       <c r="D12" s="2">
-        <v>40180</v>
+        <v>40179</v>
       </c>
       <c r="E12" t="s">
         <v>25</v>
@@ -1455,7 +1568,7 @@
       </c>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>87</v>
       </c>
@@ -1466,7 +1579,7 @@
         <v>13</v>
       </c>
       <c r="D13" s="2">
-        <v>40181</v>
+        <v>40179</v>
       </c>
       <c r="E13" t="s">
         <v>25</v>
@@ -1477,7 +1590,7 @@
       </c>
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>88</v>
       </c>
@@ -1488,7 +1601,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="2">
-        <v>40182</v>
+        <v>40179</v>
       </c>
       <c r="E14" t="s">
         <v>25</v>
@@ -1499,7 +1612,7 @@
       </c>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>89</v>
       </c>
@@ -1510,7 +1623,7 @@
         <v>13</v>
       </c>
       <c r="D15" s="2">
-        <v>40183</v>
+        <v>40179</v>
       </c>
       <c r="E15" t="s">
         <v>25</v>
@@ -1521,7 +1634,7 @@
       </c>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -1539,7 +1652,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>90</v>
       </c>
@@ -1557,7 +1670,7 @@
       </c>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>91</v>
       </c>
@@ -1575,7 +1688,7 @@
       </c>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>92</v>
       </c>
@@ -1593,7 +1706,7 @@
       </c>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>93</v>
       </c>
@@ -1611,7 +1724,7 @@
       </c>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>94</v>
       </c>
@@ -1627,7 +1740,7 @@
       </c>
       <c r="I21" s="7"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>95</v>
       </c>
@@ -1643,7 +1756,7 @@
       </c>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>96</v>
       </c>
@@ -1659,7 +1772,7 @@
       </c>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>97</v>
       </c>
@@ -1675,7 +1788,7 @@
       </c>
       <c r="I24" s="7"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>98</v>
       </c>
@@ -1691,7 +1804,7 @@
       </c>
       <c r="I25" s="7"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1711,7 +1824,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>99</v>
       </c>
@@ -1733,7 +1846,7 @@
       </c>
       <c r="I27" s="7"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>100</v>
       </c>
@@ -1755,7 +1868,7 @@
       </c>
       <c r="I28" s="7"/>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>101</v>
       </c>
@@ -1777,7 +1890,7 @@
       </c>
       <c r="I29" s="7"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>102</v>
       </c>
@@ -1799,7 +1912,7 @@
       </c>
       <c r="I30" s="7"/>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1819,7 +1932,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>103</v>
       </c>
@@ -1841,7 +1954,7 @@
       </c>
       <c r="I32" s="7"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>104</v>
       </c>
@@ -1863,7 +1976,7 @@
       </c>
       <c r="I33" s="7"/>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>105</v>
       </c>
@@ -1885,7 +1998,7 @@
       </c>
       <c r="I34" s="7"/>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>106</v>
       </c>
@@ -1907,7 +2020,7 @@
       </c>
       <c r="I35" s="7"/>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>26</v>
       </c>
@@ -1927,7 +2040,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>107</v>
       </c>
@@ -1949,7 +2062,7 @@
       </c>
       <c r="I37" s="7"/>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>108</v>
       </c>
@@ -1971,7 +2084,7 @@
       </c>
       <c r="I38" s="7"/>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>109</v>
       </c>
@@ -1993,7 +2106,7 @@
       </c>
       <c r="I39" s="7"/>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>110</v>
       </c>
@@ -2015,7 +2128,7 @@
       </c>
       <c r="I40" s="7"/>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>32</v>
       </c>
@@ -2035,7 +2148,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>34</v>
       </c>
@@ -2055,7 +2168,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>36</v>
       </c>
@@ -2075,7 +2188,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>38</v>
       </c>
@@ -2095,7 +2208,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>40</v>
       </c>
@@ -2115,7 +2228,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>42</v>
       </c>
@@ -2135,7 +2248,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>44</v>
       </c>
@@ -2155,7 +2268,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -2175,7 +2288,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -2195,7 +2308,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -2215,7 +2328,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -2235,7 +2348,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>54</v>
       </c>
@@ -2255,7 +2368,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -2275,7 +2388,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>58</v>
       </c>
@@ -2295,7 +2408,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>71</v>
       </c>
@@ -2315,7 +2428,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>72</v>
       </c>
@@ -2335,7 +2448,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>68</v>
       </c>
@@ -2382,9 +2495,9 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
       <c r="B1" s="1" t="str">
         <f>A2</f>
@@ -2419,13 +2532,13 @@
         <v>DoFVC</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="8"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>15</v>
       </c>
@@ -2434,7 +2547,7 @@
       </c>
       <c r="C3" s="8"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>17</v>
       </c>
@@ -2446,7 +2559,7 @@
       </c>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>70</v>
       </c>
@@ -2461,7 +2574,7 @@
       </c>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>62</v>
       </c>
@@ -2472,7 +2585,7 @@
       <c r="D6" s="4"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>31</v>
       </c>
@@ -2484,7 +2597,7 @@
       </c>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>33</v>
       </c>
@@ -2499,7 +2612,7 @@
       </c>
       <c r="H8" s="8"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
Kolommen toegevoegd voor ECAS en MRI
</commit_message>
<xml_diff>
--- a/Data/Format_v1.xlsx
+++ b/Data/Format_v1.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28600" windowHeight="15940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$57</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$100</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -313,7 +313,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="230">
   <si>
     <t>Original</t>
   </si>
@@ -739,13 +739,277 @@
   </si>
   <si>
     <t>ALS number</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>FU2: Language</t>
+  </si>
+  <si>
+    <t>FU3: Language</t>
+  </si>
+  <si>
+    <t>FU4: Language</t>
+  </si>
+  <si>
+    <t>FU5: Language</t>
+  </si>
+  <si>
+    <t>Fluency Free + Fixed</t>
+  </si>
+  <si>
+    <t>FU2: Fluency_Free + Fixed</t>
+  </si>
+  <si>
+    <t>FU3: Fluency_Free + Fixed</t>
+  </si>
+  <si>
+    <t>FU4: Fluency_Free + Fixed</t>
+  </si>
+  <si>
+    <t>FU5: Fluency_Free + Fixed</t>
+  </si>
+  <si>
+    <t>Executive</t>
+  </si>
+  <si>
+    <t>FU2: Executive</t>
+  </si>
+  <si>
+    <t>FU3: Executive</t>
+  </si>
+  <si>
+    <t>FU4: Executive</t>
+  </si>
+  <si>
+    <t>FU5: Executive</t>
+  </si>
+  <si>
+    <t>Memory</t>
+  </si>
+  <si>
+    <t>FU2: Memory</t>
+  </si>
+  <si>
+    <t>FU3: Memory</t>
+  </si>
+  <si>
+    <t>FU4: Memory</t>
+  </si>
+  <si>
+    <t>FU5: Memory</t>
+  </si>
+  <si>
+    <t>Visuospatial</t>
+  </si>
+  <si>
+    <t>FU2: Visuospatial</t>
+  </si>
+  <si>
+    <t>FU3: Visuospatial</t>
+  </si>
+  <si>
+    <t>FU4: Visuospatial</t>
+  </si>
+  <si>
+    <t>FU5: Visuospatial</t>
+  </si>
+  <si>
+    <t>FollowUp1_datum_scan</t>
+  </si>
+  <si>
+    <t>FollowUp2_datum_scan</t>
+  </si>
+  <si>
+    <t>FollowUp3_datum_scan</t>
+  </si>
+  <si>
+    <t>FollowUp4_datum_scan</t>
+  </si>
+  <si>
+    <t>FollowUp5_datum_scan</t>
+  </si>
+  <si>
+    <t>FollowUp6_datum_scan</t>
+  </si>
+  <si>
+    <t>FollowUp1_T1</t>
+  </si>
+  <si>
+    <t>FollowUp2_T1</t>
+  </si>
+  <si>
+    <t>FollowUp3_T1</t>
+  </si>
+  <si>
+    <t>FollowUp4_T1</t>
+  </si>
+  <si>
+    <t>FollowUp5_T1</t>
+  </si>
+  <si>
+    <t>FollowUp6_T1</t>
+  </si>
+  <si>
+    <t>FollowUp1_DTI</t>
+  </si>
+  <si>
+    <t>FollowUp2_DTI</t>
+  </si>
+  <si>
+    <t>FollowUp3_DTI</t>
+  </si>
+  <si>
+    <t>FollowUp4_DTI</t>
+  </si>
+  <si>
+    <t>FollowUp5_DTI</t>
+  </si>
+  <si>
+    <t>FollowUp6_DTI</t>
+  </si>
+  <si>
+    <t>ECAS_language1</t>
+  </si>
+  <si>
+    <t>ECAS_language2</t>
+  </si>
+  <si>
+    <t>ECAS_language3</t>
+  </si>
+  <si>
+    <t>ECAS_language4</t>
+  </si>
+  <si>
+    <t>ECAS_language5</t>
+  </si>
+  <si>
+    <t>ECAS_fluency1</t>
+  </si>
+  <si>
+    <t>ECAS_fluency2</t>
+  </si>
+  <si>
+    <t>ECAS_fluency3</t>
+  </si>
+  <si>
+    <t>ECAS_fluency4</t>
+  </si>
+  <si>
+    <t>ECAS_fluency5</t>
+  </si>
+  <si>
+    <t>ECAS_executive1</t>
+  </si>
+  <si>
+    <t>ECAS_executive2</t>
+  </si>
+  <si>
+    <t>ECAS_executive3</t>
+  </si>
+  <si>
+    <t>ECAS_executive4</t>
+  </si>
+  <si>
+    <t>ECAS_executive5</t>
+  </si>
+  <si>
+    <t>ECAS_memory1</t>
+  </si>
+  <si>
+    <t>ECAS_memory2</t>
+  </si>
+  <si>
+    <t>ECAS_memory3</t>
+  </si>
+  <si>
+    <t>ECAS_memory4</t>
+  </si>
+  <si>
+    <t>ECAS_memory5</t>
+  </si>
+  <si>
+    <t>ECAS_visuosp1</t>
+  </si>
+  <si>
+    <t>ECAS_visuosp2</t>
+  </si>
+  <si>
+    <t>ECAS_visuosp3</t>
+  </si>
+  <si>
+    <t>ECAS_visuosp4</t>
+  </si>
+  <si>
+    <t>ECAS_visuosp5</t>
+  </si>
+  <si>
+    <t>DoMRI1</t>
+  </si>
+  <si>
+    <t>DoMRI2</t>
+  </si>
+  <si>
+    <t>DoMRI3</t>
+  </si>
+  <si>
+    <t>DoMRI4</t>
+  </si>
+  <si>
+    <t>DoMRI5</t>
+  </si>
+  <si>
+    <t>DoMRI6</t>
+  </si>
+  <si>
+    <t>MRI_T1pres1</t>
+  </si>
+  <si>
+    <t>MRI_T1pres2</t>
+  </si>
+  <si>
+    <t>MRI_T1pres3</t>
+  </si>
+  <si>
+    <t>MRI_T1pres4</t>
+  </si>
+  <si>
+    <t>MRI_T1pres5</t>
+  </si>
+  <si>
+    <t>MRI_T1pres6</t>
+  </si>
+  <si>
+    <t>MRI_DTIpres1</t>
+  </si>
+  <si>
+    <t>MRI_DTIpres2</t>
+  </si>
+  <si>
+    <t>MRI_DTIpres3</t>
+  </si>
+  <si>
+    <t>MRI_DTIpres4</t>
+  </si>
+  <si>
+    <t>MRI_DTIpres5</t>
+  </si>
+  <si>
+    <t>MRI_DTIpres6</t>
+  </si>
+  <si>
+    <t>Yes|No</t>
+  </si>
+  <si>
+    <t>MRI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -776,17 +1040,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <sz val="9"/>
@@ -834,6 +1087,21 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)_x0000_"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)_x0000_"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri (Body)_x0000_"/>
     </font>
   </fonts>
   <fills count="4">
@@ -910,18 +1178,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1303,26 +1575,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J57"/>
+  <dimension ref="A1:J100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="50.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="50.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.33203125" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1353,1127 +1626,2049 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:10">
+      <c r="A2" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:10">
+      <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:10">
+      <c r="A4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="12">
         <v>367</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:10">
+      <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="12">
         <v>18264</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:10">
+      <c r="A6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="12">
         <v>18264</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:10">
+      <c r="A7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="12">
         <v>29221</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:10">
+      <c r="A8" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="12">
         <v>29221</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:10">
+      <c r="A9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="12">
         <v>40179</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="H11" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="12">
         <v>40179</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="5"/>
-      <c r="H12" t="s">
-        <v>80</v>
-      </c>
-      <c r="I12" s="7"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="F12" s="11"/>
+      <c r="H12" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="12">
         <v>40179</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="5"/>
-      <c r="H13" t="s">
-        <v>80</v>
-      </c>
-      <c r="I13" s="7"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="F13" s="11"/>
+      <c r="H13" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="12">
         <v>40179</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="5"/>
-      <c r="H14" t="s">
-        <v>80</v>
-      </c>
-      <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="F14" s="11"/>
+      <c r="H14" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="12">
         <v>40179</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="5"/>
-      <c r="H15" t="s">
-        <v>80</v>
-      </c>
-      <c r="I15" s="7"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="F15" s="11"/>
+      <c r="H15" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="F16" t="s">
+      <c r="D16" s="12"/>
+      <c r="F16" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H16" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="H16" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H17" t="s">
-        <v>80</v>
-      </c>
-      <c r="I17" s="7"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="H17" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H18" t="s">
-        <v>80</v>
-      </c>
-      <c r="I18" s="7"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="H18" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H19" t="s">
-        <v>80</v>
-      </c>
-      <c r="I19" s="7"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="H19" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H20" t="s">
-        <v>80</v>
-      </c>
-      <c r="I20" s="7"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="H20" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F21" s="5"/>
-      <c r="H21" t="s">
-        <v>80</v>
-      </c>
-      <c r="I21" s="7"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="F21" s="11"/>
+      <c r="H21" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F22" s="5"/>
-      <c r="H22" t="s">
-        <v>80</v>
-      </c>
-      <c r="I22" s="7"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="F22" s="11"/>
+      <c r="H22" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="5"/>
-      <c r="H23" t="s">
-        <v>80</v>
-      </c>
-      <c r="I23" s="7"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="F23" s="11"/>
+      <c r="H23" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="5"/>
-      <c r="H24" t="s">
-        <v>80</v>
-      </c>
-      <c r="I24" s="7"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="F24" s="11"/>
+      <c r="H24" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F25" s="5"/>
-      <c r="H25" t="s">
-        <v>80</v>
-      </c>
-      <c r="I25" s="7"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="F25" s="11"/>
+      <c r="H25" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C26" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" s="5">
-        <v>0</v>
-      </c>
-      <c r="E26" s="5">
+      <c r="C26" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="11">
+        <v>0</v>
+      </c>
+      <c r="E26" s="11">
         <v>100</v>
       </c>
-      <c r="H26" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="H26" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="C27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="5">
-        <v>0</v>
-      </c>
-      <c r="E27" s="5">
+      <c r="C27" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="11">
+        <v>0</v>
+      </c>
+      <c r="E27" s="11">
         <v>100</v>
       </c>
-      <c r="F27" s="5"/>
-      <c r="H27" t="s">
-        <v>80</v>
-      </c>
-      <c r="I27" s="7"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="F27" s="11"/>
+      <c r="H27" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C28" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="5">
-        <v>0</v>
-      </c>
-      <c r="E28" s="5">
+      <c r="C28" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="11">
+        <v>0</v>
+      </c>
+      <c r="E28" s="11">
         <v>100</v>
       </c>
-      <c r="F28" s="5"/>
-      <c r="H28" t="s">
-        <v>80</v>
-      </c>
-      <c r="I28" s="7"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="F28" s="11"/>
+      <c r="H28" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="C29" t="s">
-        <v>27</v>
-      </c>
-      <c r="D29" s="5">
-        <v>0</v>
-      </c>
-      <c r="E29" s="5">
+      <c r="C29" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="11">
+        <v>0</v>
+      </c>
+      <c r="E29" s="11">
         <v>100</v>
       </c>
-      <c r="F29" s="5"/>
-      <c r="H29" t="s">
-        <v>80</v>
-      </c>
-      <c r="I29" s="7"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="F29" s="11"/>
+      <c r="H29" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I29" s="3"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="C30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D30" s="5">
-        <v>0</v>
-      </c>
-      <c r="E30" s="5">
+      <c r="C30" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="11">
+        <v>0</v>
+      </c>
+      <c r="E30" s="11">
         <v>100</v>
       </c>
-      <c r="F30" s="5"/>
-      <c r="H30" t="s">
-        <v>80</v>
-      </c>
-      <c r="I30" s="7"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="F30" s="11"/>
+      <c r="H30" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="C31" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" s="5">
-        <v>0</v>
-      </c>
-      <c r="E31" s="5">
+      <c r="C31" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="11">
+        <v>0</v>
+      </c>
+      <c r="E31" s="11">
         <v>36</v>
       </c>
-      <c r="H31" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="H31" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="C32" t="s">
-        <v>27</v>
-      </c>
-      <c r="D32" s="5">
-        <v>0</v>
-      </c>
-      <c r="E32" s="5">
+      <c r="C32" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="11">
+        <v>0</v>
+      </c>
+      <c r="E32" s="11">
         <v>36</v>
       </c>
-      <c r="F32" s="5"/>
-      <c r="H32" t="s">
-        <v>80</v>
-      </c>
-      <c r="I32" s="7"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="F32" s="11"/>
+      <c r="H32" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I32" s="3"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="C33" t="s">
-        <v>27</v>
-      </c>
-      <c r="D33" s="5">
-        <v>0</v>
-      </c>
-      <c r="E33" s="5">
+      <c r="C33" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="11">
+        <v>0</v>
+      </c>
+      <c r="E33" s="11">
         <v>36</v>
       </c>
-      <c r="F33" s="5"/>
-      <c r="H33" t="s">
-        <v>80</v>
-      </c>
-      <c r="I33" s="7"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="F33" s="11"/>
+      <c r="H33" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I33" s="3"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C34" t="s">
-        <v>27</v>
-      </c>
-      <c r="D34" s="5">
-        <v>0</v>
-      </c>
-      <c r="E34" s="5">
+      <c r="C34" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="11">
+        <v>0</v>
+      </c>
+      <c r="E34" s="11">
         <v>36</v>
       </c>
-      <c r="F34" s="5"/>
-      <c r="H34" t="s">
-        <v>80</v>
-      </c>
-      <c r="I34" s="7"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="F34" s="11"/>
+      <c r="H34" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I34" s="3"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C35" t="s">
-        <v>27</v>
-      </c>
-      <c r="D35" s="5">
-        <v>0</v>
-      </c>
-      <c r="E35" s="5">
+      <c r="C35" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="11">
+        <v>0</v>
+      </c>
+      <c r="E35" s="11">
         <v>36</v>
       </c>
-      <c r="F35" s="5"/>
-      <c r="H35" t="s">
-        <v>80</v>
-      </c>
-      <c r="I35" s="7"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="F35" s="11"/>
+      <c r="H35" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I35" s="3"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="C36" t="s">
-        <v>27</v>
-      </c>
-      <c r="D36" s="5">
-        <v>0</v>
-      </c>
-      <c r="E36" s="5">
+      <c r="C36" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="11">
+        <v>0</v>
+      </c>
+      <c r="E36" s="11">
         <v>136</v>
       </c>
-      <c r="H36" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="H36" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C37" t="s">
-        <v>27</v>
-      </c>
-      <c r="D37" s="5">
-        <v>0</v>
-      </c>
-      <c r="E37" s="5">
+      <c r="C37" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" s="11">
+        <v>0</v>
+      </c>
+      <c r="E37" s="11">
         <v>136</v>
       </c>
-      <c r="F37" s="5"/>
-      <c r="H37" t="s">
-        <v>80</v>
-      </c>
-      <c r="I37" s="7"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="F37" s="11"/>
+      <c r="H37" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I37" s="3"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="C38" t="s">
-        <v>27</v>
-      </c>
-      <c r="D38" s="5">
-        <v>0</v>
-      </c>
-      <c r="E38" s="5">
+      <c r="C38" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D38" s="11">
+        <v>0</v>
+      </c>
+      <c r="E38" s="11">
         <v>136</v>
       </c>
-      <c r="F38" s="5"/>
-      <c r="H38" t="s">
-        <v>80</v>
-      </c>
-      <c r="I38" s="7"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="F38" s="11"/>
+      <c r="H38" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I38" s="3"/>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="C39" t="s">
-        <v>27</v>
-      </c>
-      <c r="D39" s="5">
-        <v>0</v>
-      </c>
-      <c r="E39" s="5">
+      <c r="C39" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="11">
+        <v>0</v>
+      </c>
+      <c r="E39" s="11">
         <v>136</v>
       </c>
-      <c r="F39" s="5"/>
-      <c r="H39" t="s">
-        <v>80</v>
-      </c>
-      <c r="I39" s="7"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="F39" s="11"/>
+      <c r="H39" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I39" s="3"/>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C40" t="s">
-        <v>27</v>
-      </c>
-      <c r="D40" s="5">
-        <v>0</v>
-      </c>
-      <c r="E40" s="5">
+      <c r="C40" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" s="11">
+        <v>0</v>
+      </c>
+      <c r="E40" s="11">
         <v>136</v>
       </c>
-      <c r="F40" s="5"/>
-      <c r="H40" t="s">
-        <v>80</v>
-      </c>
-      <c r="I40" s="7"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="F40" s="11"/>
+      <c r="H40" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I40" s="3"/>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41" s="11">
+        <v>0</v>
+      </c>
+      <c r="E41" s="11">
+        <v>28</v>
+      </c>
+      <c r="F41" s="11"/>
+      <c r="H41" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I41" s="3"/>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42" s="11">
+        <v>0</v>
+      </c>
+      <c r="E42" s="11">
+        <v>28</v>
+      </c>
+      <c r="F42" s="11"/>
+      <c r="H42" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I42" s="3"/>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D43" s="11">
+        <v>0</v>
+      </c>
+      <c r="E43" s="11">
+        <v>28</v>
+      </c>
+      <c r="F43" s="11"/>
+      <c r="H43" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I43" s="3"/>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" s="11">
+        <v>0</v>
+      </c>
+      <c r="E44" s="11">
+        <v>28</v>
+      </c>
+      <c r="F44" s="11"/>
+      <c r="H44" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I44" s="3"/>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D45" s="11">
+        <v>0</v>
+      </c>
+      <c r="E45" s="11">
+        <v>28</v>
+      </c>
+      <c r="F45" s="11"/>
+      <c r="H45" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I45" s="3"/>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D46" s="11">
+        <v>0</v>
+      </c>
+      <c r="E46" s="11">
+        <v>24</v>
+      </c>
+      <c r="F46" s="11"/>
+      <c r="H46" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I46" s="3"/>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D47" s="11">
+        <v>0</v>
+      </c>
+      <c r="E47" s="11">
+        <v>24</v>
+      </c>
+      <c r="F47" s="11"/>
+      <c r="H47" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I47" s="3"/>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D48" s="11">
+        <v>0</v>
+      </c>
+      <c r="E48" s="11">
+        <v>24</v>
+      </c>
+      <c r="F48" s="11"/>
+      <c r="H48" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I48" s="3"/>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D49" s="11">
+        <v>0</v>
+      </c>
+      <c r="E49" s="11">
+        <v>24</v>
+      </c>
+      <c r="F49" s="11"/>
+      <c r="H49" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I49" s="3"/>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D50" s="11">
+        <v>0</v>
+      </c>
+      <c r="E50" s="11">
+        <v>24</v>
+      </c>
+      <c r="F50" s="11"/>
+      <c r="H50" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I50" s="3"/>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D51" s="11">
+        <v>0</v>
+      </c>
+      <c r="E51" s="11">
+        <v>48</v>
+      </c>
+      <c r="F51" s="11"/>
+      <c r="H51" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I51" s="3"/>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D52" s="11">
+        <v>0</v>
+      </c>
+      <c r="E52" s="11">
+        <v>48</v>
+      </c>
+      <c r="F52" s="11"/>
+      <c r="H52" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I52" s="3"/>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D53" s="11">
+        <v>0</v>
+      </c>
+      <c r="E53" s="11">
+        <v>48</v>
+      </c>
+      <c r="F53" s="11"/>
+      <c r="H53" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I53" s="3"/>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D54" s="11">
+        <v>0</v>
+      </c>
+      <c r="E54" s="11">
+        <v>48</v>
+      </c>
+      <c r="F54" s="11"/>
+      <c r="H54" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I54" s="3"/>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D55" s="11">
+        <v>0</v>
+      </c>
+      <c r="E55" s="11">
+        <v>48</v>
+      </c>
+      <c r="F55" s="11"/>
+      <c r="H55" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I55" s="3"/>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D56" s="11">
+        <v>0</v>
+      </c>
+      <c r="E56" s="11">
+        <v>24</v>
+      </c>
+      <c r="F56" s="11"/>
+      <c r="H56" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I56" s="3"/>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D57" s="11">
+        <v>0</v>
+      </c>
+      <c r="E57" s="11">
+        <v>24</v>
+      </c>
+      <c r="F57" s="11"/>
+      <c r="H57" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I57" s="3"/>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D58" s="11">
+        <v>0</v>
+      </c>
+      <c r="E58" s="11">
+        <v>24</v>
+      </c>
+      <c r="F58" s="11"/>
+      <c r="H58" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I58" s="3"/>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D59" s="11">
+        <v>0</v>
+      </c>
+      <c r="E59" s="11">
+        <v>24</v>
+      </c>
+      <c r="F59" s="11"/>
+      <c r="H59" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I59" s="3"/>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D60" s="11">
+        <v>0</v>
+      </c>
+      <c r="E60" s="11">
+        <v>24</v>
+      </c>
+      <c r="F60" s="11"/>
+      <c r="H60" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I60" s="3"/>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D61" s="11">
+        <v>0</v>
+      </c>
+      <c r="E61" s="11">
+        <v>12</v>
+      </c>
+      <c r="F61" s="11"/>
+      <c r="H61" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I61" s="3"/>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D62" s="11">
+        <v>0</v>
+      </c>
+      <c r="E62" s="11">
+        <v>12</v>
+      </c>
+      <c r="F62" s="11"/>
+      <c r="H62" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I62" s="3"/>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D63" s="11">
+        <v>0</v>
+      </c>
+      <c r="E63" s="11">
+        <v>12</v>
+      </c>
+      <c r="F63" s="11"/>
+      <c r="H63" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I63" s="3"/>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D64" s="11">
+        <v>0</v>
+      </c>
+      <c r="E64" s="11">
+        <v>12</v>
+      </c>
+      <c r="F64" s="11"/>
+      <c r="H64" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I64" s="3"/>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D65" s="11">
+        <v>0</v>
+      </c>
+      <c r="E65" s="11">
+        <v>12</v>
+      </c>
+      <c r="F65" s="11"/>
+      <c r="H65" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I65" s="3"/>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D66" s="13">
+        <v>39814</v>
+      </c>
+      <c r="E66" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F66" s="11"/>
+      <c r="H66" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="I66" s="3"/>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D67" s="13">
+        <v>39814</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F67" s="11"/>
+      <c r="H67" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="I67" s="3"/>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D68" s="13">
+        <v>39814</v>
+      </c>
+      <c r="E68" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F68" s="11"/>
+      <c r="H68" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="I68" s="3"/>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D69" s="13">
+        <v>39814</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F69" s="11"/>
+      <c r="H69" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="I69" s="3"/>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D70" s="13">
+        <v>39814</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F70" s="11"/>
+      <c r="H70" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="I70" s="3"/>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D71" s="13">
+        <v>39814</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F71" s="11"/>
+      <c r="H71" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="I71" s="3"/>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D72" s="11"/>
+      <c r="E72" s="11"/>
+      <c r="F72" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="H72" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="I72" s="3"/>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D73" s="11"/>
+      <c r="E73" s="11"/>
+      <c r="F73" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="H73" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="I73" s="3"/>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74" s="11"/>
+      <c r="E74" s="11"/>
+      <c r="F74" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="H74" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="I74" s="3"/>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D75" s="11"/>
+      <c r="E75" s="11"/>
+      <c r="F75" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="H75" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="I75" s="3"/>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76" s="11"/>
+      <c r="E76" s="11"/>
+      <c r="F76" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="H76" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="I76" s="3"/>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77" s="11"/>
+      <c r="E77" s="11"/>
+      <c r="F77" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="H77" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="I77" s="3"/>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D78" s="11"/>
+      <c r="E78" s="11"/>
+      <c r="F78" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="H78" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="I78" s="3"/>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="A79" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D79" s="11"/>
+      <c r="E79" s="11"/>
+      <c r="F79" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="H79" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="I79" s="3"/>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D80" s="11"/>
+      <c r="E80" s="11"/>
+      <c r="F80" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="H80" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="I80" s="3"/>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="A81" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D81" s="11"/>
+      <c r="E81" s="11"/>
+      <c r="F81" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="H81" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="I81" s="3"/>
+    </row>
+    <row r="82" spans="1:9">
+      <c r="A82" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D82" s="11"/>
+      <c r="E82" s="11"/>
+      <c r="F82" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="H82" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="I82" s="3"/>
+    </row>
+    <row r="83" spans="1:9">
+      <c r="A83" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D83" s="11"/>
+      <c r="E83" s="11"/>
+      <c r="F83" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="H83" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="I83" s="3"/>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="A84" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B84" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C84" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D84" s="12">
         <v>32874</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E84" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H84" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="85" spans="1:9">
+      <c r="A85" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B85" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C42" t="s">
-        <v>27</v>
-      </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42">
+      <c r="C85" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D85" s="7">
+        <v>0</v>
+      </c>
+      <c r="E85" s="7">
         <v>4</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H85" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="86" spans="1:9">
+      <c r="A86" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B86" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C43" t="s">
-        <v>27</v>
-      </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="E43">
+      <c r="C86" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D86" s="7">
+        <v>0</v>
+      </c>
+      <c r="E86" s="7">
         <v>4</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H86" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="87" spans="1:9">
+      <c r="A87" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B87" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C44" t="s">
-        <v>27</v>
-      </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-      <c r="E44">
+      <c r="C87" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D87" s="7">
+        <v>0</v>
+      </c>
+      <c r="E87" s="7">
         <v>4</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H87" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="88" spans="1:9">
+      <c r="A88" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B88" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C45" t="s">
-        <v>27</v>
-      </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="E45">
+      <c r="C88" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D88" s="7">
+        <v>0</v>
+      </c>
+      <c r="E88" s="7">
         <v>4</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H88" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="89" spans="1:9">
+      <c r="A89" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B89" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C46" t="s">
-        <v>27</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46">
+      <c r="C89" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D89" s="7">
+        <v>0</v>
+      </c>
+      <c r="E89" s="7">
         <v>4</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H89" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="90" spans="1:9">
+      <c r="A90" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B90" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C47" t="s">
-        <v>27</v>
-      </c>
-      <c r="D47">
-        <v>0</v>
-      </c>
-      <c r="E47">
+      <c r="C90" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D90" s="7">
+        <v>0</v>
+      </c>
+      <c r="E90" s="7">
         <v>4</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H90" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+    <row r="91" spans="1:9">
+      <c r="A91" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B91" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C48" t="s">
-        <v>27</v>
-      </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
-      <c r="E48">
+      <c r="C91" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D91" s="7">
+        <v>0</v>
+      </c>
+      <c r="E91" s="7">
         <v>4</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H91" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="92" spans="1:9">
+      <c r="A92" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B92" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C49" t="s">
-        <v>27</v>
-      </c>
-      <c r="D49">
-        <v>0</v>
-      </c>
-      <c r="E49">
+      <c r="C92" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D92" s="7">
+        <v>0</v>
+      </c>
+      <c r="E92" s="7">
         <v>4</v>
       </c>
-      <c r="H49" t="s">
+      <c r="H92" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="93" spans="1:9">
+      <c r="A93" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B93" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C50" t="s">
-        <v>27</v>
-      </c>
-      <c r="D50">
-        <v>0</v>
-      </c>
-      <c r="E50">
+      <c r="C93" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D93" s="7">
+        <v>0</v>
+      </c>
+      <c r="E93" s="7">
         <v>4</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H93" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="94" spans="1:9">
+      <c r="A94" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B94" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C51" t="s">
-        <v>27</v>
-      </c>
-      <c r="D51">
-        <v>0</v>
-      </c>
-      <c r="E51">
+      <c r="C94" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D94" s="7">
+        <v>0</v>
+      </c>
+      <c r="E94" s="7">
         <v>4</v>
       </c>
-      <c r="H51" t="s">
+      <c r="H94" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+    <row r="95" spans="1:9">
+      <c r="A95" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B95" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C52" t="s">
-        <v>27</v>
-      </c>
-      <c r="D52">
-        <v>0</v>
-      </c>
-      <c r="E52">
+      <c r="C95" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D95" s="7">
+        <v>0</v>
+      </c>
+      <c r="E95" s="7">
         <v>4</v>
       </c>
-      <c r="H52" t="s">
+      <c r="H95" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="96" spans="1:9">
+      <c r="A96" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B96" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C53" t="s">
-        <v>27</v>
-      </c>
-      <c r="D53">
-        <v>0</v>
-      </c>
-      <c r="E53">
+      <c r="C96" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D96" s="7">
+        <v>0</v>
+      </c>
+      <c r="E96" s="7">
         <v>4</v>
       </c>
-      <c r="H53" t="s">
+      <c r="H96" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="97" spans="1:9">
+      <c r="A97" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B97" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C54" t="s">
-        <v>27</v>
-      </c>
-      <c r="D54">
-        <v>0</v>
-      </c>
-      <c r="E54">
+      <c r="C97" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D97" s="7">
+        <v>0</v>
+      </c>
+      <c r="E97" s="7">
         <v>4</v>
       </c>
-      <c r="H54" t="s">
+      <c r="H97" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" s="6" t="s">
+    <row r="98" spans="1:9">
+      <c r="A98" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B98" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C98" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D55" s="2">
+      <c r="D98" s="12">
         <v>29221</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E98" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H55" t="s">
+      <c r="H98" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="99" spans="1:9">
+      <c r="A99" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B99" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C56" t="s">
-        <v>27</v>
-      </c>
-      <c r="D56">
+      <c r="C99" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D99" s="7">
         <v>20</v>
       </c>
-      <c r="E56">
+      <c r="E99" s="7">
         <v>200</v>
       </c>
-      <c r="H56" t="s">
+      <c r="H99" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="100" spans="1:9">
+      <c r="A100" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B100" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C100" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="D100" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E57" s="4" t="s">
+      <c r="E100" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F57" s="4" t="s">
+      <c r="F100" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G57" s="4" t="s">
+      <c r="G100" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="H57" s="4" t="s">
+      <c r="H100" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="I57" s="4"/>
+      <c r="I100" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2495,10 +3690,10 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="4"/>
+    <row r="1" spans="1:9">
+      <c r="A1" s="2"/>
       <c r="B1" s="1" t="str">
         <f>A2</f>
         <v>DoB</v>
@@ -2532,23 +3727,23 @@
         <v>DoFVC</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:9">
+      <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="8"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="B2" s="4"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B3">
         <v>-1</v>
       </c>
-      <c r="C3" s="8"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B4">
@@ -2557,10 +3752,10 @@
       <c r="C4">
         <v>-1</v>
       </c>
-      <c r="D4" s="8"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="5" t="s">
         <v>70</v>
       </c>
       <c r="B5">
@@ -2572,21 +3767,21 @@
       <c r="D5">
         <v>-1</v>
       </c>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B6">
         <v>-1</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B7">
@@ -2595,10 +3790,10 @@
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B8">
@@ -2610,10 +3805,10 @@
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="H8" s="8"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="6" t="s">
         <v>73</v>
       </c>
       <c r="B9">
@@ -2622,7 +3817,7 @@
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="I9" s="8"/>
+      <c r="I9" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
DoMRI toegevoegd aan Sheet2
</commit_message>
<xml_diff>
--- a/Data/Format_v1.xlsx
+++ b/Data/Format_v1.xlsx
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$100</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -234,7 +234,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="231">
   <si>
     <t>Original</t>
   </si>
@@ -924,6 +924,9 @@
   </si>
   <si>
     <t>MRI</t>
+  </si>
+  <si>
+    <t>DoMRI</t>
   </si>
 </sst>
 </file>
@@ -1047,8 +1050,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1108,7 +1113,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1130,6 +1135,7 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1151,6 +1157,7 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3597,15 +3604,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="2"/>
       <c r="B1" s="1" t="str">
         <f>A2</f>
@@ -3639,14 +3646,18 @@
         <f>A9</f>
         <v>DoFVC</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="str">
+        <f>A10</f>
+        <v>DoMRI</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
@@ -3655,7 +3666,7 @@
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
@@ -3667,7 +3678,7 @@
       </c>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="5" t="s">
         <v>70</v>
       </c>
@@ -3682,7 +3693,7 @@
       </c>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" s="5" t="s">
         <v>62</v>
       </c>
@@ -3693,7 +3704,7 @@
       <c r="D6" s="2"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" s="5" t="s">
         <v>31</v>
       </c>
@@ -3705,7 +3716,7 @@
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" s="5" t="s">
         <v>33</v>
       </c>
@@ -3720,7 +3731,7 @@
       </c>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" s="5" t="s">
         <v>73</v>
       </c>
@@ -3731,6 +3742,18 @@
         <v>1</v>
       </c>
       <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B10">
+        <v>-1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="J10" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Minor change in sheet 2, DoALSFTDQ can occur after DoDeath
</commit_message>
<xml_diff>
--- a/Data/Format_v1.xlsx
+++ b/Data/Format_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/htan4/Documents/Rprojects/ResearchR/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{49EEF06C-E592-F049-BEC4-C49FD32C3876}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{DDA21A61-B7F2-9743-800F-FFDA9480F9A4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25020" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="25020" windowHeight="15940" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2397,8 +2397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
-      <selection activeCell="K202" sqref="K202"/>
+    <sheetView topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="J231" sqref="J203:J231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7165,8 +7165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7337,9 +7337,6 @@
       </c>
       <c r="C12">
         <v>-1</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>